<commit_message>
Login test and fix general tab with assert
</commit_message>
<xml_diff>
--- a/src/test/testData/TestData.xlsx
+++ b/src/test/testData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.tanasijevic\IdeaProjects\sCore-Automation\src\test\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E639C83-D76F-47BF-86D6-F97E2A26EC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8EF405-3E4B-4862-85A2-CE6FEE59695F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="290" xr2:uid="{446C2EEA-32A6-4059-8605-697140F2B872}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="171">
   <si>
     <t>TC ID</t>
   </si>
@@ -519,6 +519,39 @@
   </si>
   <si>
     <t>EUR</t>
+  </si>
+  <si>
+    <t>Drzava</t>
+  </si>
+  <si>
+    <t>Metod placanja</t>
+  </si>
+  <si>
+    <t>Dinamika placanja</t>
+  </si>
+  <si>
+    <t>Kvartalno</t>
+  </si>
+  <si>
+    <t>Trajni nalog</t>
+  </si>
+  <si>
+    <t>Administrativna zabrana</t>
+  </si>
+  <si>
+    <t>Nalog za uplatu premije</t>
+  </si>
+  <si>
+    <t>Doživotno</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>BANCA INTESA AD BEOGRAD</t>
+  </si>
+  <si>
+    <t>Riziko</t>
   </si>
 </sst>
 </file>
@@ -981,19 +1014,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A231167-7B41-45C2-955B-DBFB6AABD467}">
-  <dimension ref="A1:AW15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" style="9" customWidth="1"/>
     <col min="6" max="6" width="11.08984375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7265625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.54296875" style="9" bestFit="1" customWidth="1"/>
@@ -1002,52 +1035,13 @@
     <col min="11" max="11" width="6.26953125" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.36328125" style="9" customWidth="1"/>
     <col min="15" max="15" width="10.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="14.453125" style="9" customWidth="1"/>
-    <col min="20" max="20" width="27" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.6328125" style="9" customWidth="1"/>
-    <col min="40" max="40" width="23.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.453125" style="9" customWidth="1"/>
-    <col min="42" max="42" width="22.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="28.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="27.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="34.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="26" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="32.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18" style="9" customWidth="1"/>
-    <col min="51" max="51" width="20.26953125" style="9" customWidth="1"/>
-    <col min="52" max="65" width="8.7265625" style="9"/>
-    <col min="66" max="66" width="8.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.7265625" style="9"/>
-    <col min="69" max="69" width="19.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="71" max="16384" width="8.7265625" style="9"/>
+    <col min="16" max="16" width="14.54296875" style="9" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="4" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1070,13 +1064,13 @@
         <v>8</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>12</v>
@@ -1085,7 +1079,7 @@
         <v>13</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>15</v>
@@ -1096,41 +1090,8 @@
       <c r="P1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-    </row>
-    <row r="2" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>70</v>
       </c>
@@ -1150,7 +1111,7 @@
         <v>131</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>148</v>
@@ -1180,7 +1141,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>96</v>
       </c>
@@ -1209,16 +1170,19 @@
         <v>76</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>79</v>
+        <v>164</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>78</v>
@@ -1227,7 +1191,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>97</v>
       </c>
@@ -1241,7 +1205,7 @@
         <v>73</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>131</v>
@@ -1256,7 +1220,7 @@
         <v>76</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>159</v>
@@ -1265,7 +1229,10 @@
         <v>78</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>79</v>
+        <v>165</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>78</v>
@@ -1274,7 +1241,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>98</v>
       </c>
@@ -1303,16 +1270,19 @@
         <v>76</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>159</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>79</v>
+        <v>166</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>78</v>
@@ -1321,7 +1291,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>132</v>
       </c>
@@ -1361,6 +1331,9 @@
       <c r="M6" s="9" t="s">
         <v>79</v>
       </c>
+      <c r="N6" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="O6" s="9" t="s">
         <v>78</v>
       </c>
@@ -1368,7 +1341,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>133</v>
       </c>
@@ -1397,7 +1370,7 @@
         <v>76</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>159</v>
@@ -1406,7 +1379,10 @@
         <v>78</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>79</v>
+        <v>164</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>78</v>
@@ -1415,7 +1391,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>134</v>
       </c>
@@ -1435,7 +1411,7 @@
         <v>131</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>148</v>
@@ -1444,7 +1420,7 @@
         <v>76</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>159</v>
@@ -1453,7 +1429,10 @@
         <v>78</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>79</v>
+        <v>165</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="O8" s="9" t="s">
         <v>78</v>
@@ -1462,7 +1441,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>135</v>
       </c>
@@ -1491,16 +1470,19 @@
         <v>76</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>159</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>79</v>
+        <v>166</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="O9" s="9" t="s">
         <v>78</v>
@@ -1509,7 +1491,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>142</v>
       </c>
@@ -1549,6 +1531,9 @@
       <c r="M10" s="9" t="s">
         <v>79</v>
       </c>
+      <c r="N10" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="O10" s="9" t="s">
         <v>78</v>
       </c>
@@ -1556,7 +1541,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>143</v>
       </c>
@@ -1570,7 +1555,7 @@
         <v>73</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>141</v>
@@ -1585,16 +1570,19 @@
         <v>76</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>159</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>79</v>
+        <v>164</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="O11" s="9" t="s">
         <v>78</v>
@@ -1603,7 +1591,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1632,7 +1620,7 @@
         <v>76</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>159</v>
@@ -1641,7 +1629,10 @@
         <v>78</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>79</v>
+        <v>165</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="O12" s="9" t="s">
         <v>78</v>
@@ -1650,7 +1641,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>145</v>
       </c>
@@ -1679,16 +1670,19 @@
         <v>76</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>159</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>79</v>
+        <v>166</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="O13" s="9" t="s">
         <v>78</v>
@@ -1697,7 +1691,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>146</v>
       </c>
@@ -1737,6 +1731,9 @@
       <c r="M14" s="9" t="s">
         <v>79</v>
       </c>
+      <c r="N14" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="O14" s="9" t="s">
         <v>78</v>
       </c>
@@ -1744,7 +1741,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>147</v>
       </c>
@@ -1764,7 +1761,7 @@
         <v>141</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>148</v>
@@ -1773,16 +1770,19 @@
         <v>76</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>159</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>79</v>
+        <v>164</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>78</v>

</xml_diff>